<commit_message>
Browser utilities file updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCases.xlsx
+++ b/src/test/resources/TestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\WebDataDriven\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662D7891-C00F-4C06-9B5A-C849A84D6603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F5EC48-C577-4088-BB53-3AACBBEA5860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Smart@1234</t>
+  </si>
+  <si>
+    <t>TC_AR_002</t>
+  </si>
+  <si>
+    <t>Lady2</t>
+  </si>
+  <si>
+    <t>Raga2</t>
+  </si>
+  <si>
+    <t>raga2@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -407,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,13 +480,39 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{A694C5EB-FC5C-413C-B762-F3663F4F84FE}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{9757BE41-977C-4275-A2A1-8A34FA6E7C33}"/>
     <hyperlink ref="G2" r:id="rId3" xr:uid="{E12B992E-DBC8-4FBB-B35D-B2C7A58B949F}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{08292E5A-638F-473D-8571-F621BB9F49CC}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{551FC2F0-5B28-49AA-894A-D82692026416}"/>
+    <hyperlink ref="G3" r:id="rId6" xr:uid="{24304149-8579-485C-AE3F-43DCE0EC1158}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data provider and web tables methods added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCases.xlsx
+++ b/src/test/resources/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\WebDataDriven\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F5EC48-C577-4088-BB53-3AACBBEA5860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FB77E9-DA8B-49D1-833B-93B6B5B93D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,34 +48,34 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
-    <t>TC_AR_001</t>
-  </si>
-  <si>
-    <t>New Account Registration</t>
-  </si>
-  <si>
-    <t>Lady</t>
-  </si>
-  <si>
-    <t>Raga</t>
-  </si>
-  <si>
-    <t>raga@yopmail.com</t>
-  </si>
-  <si>
-    <t>Smart@1234</t>
-  </si>
-  <si>
-    <t>TC_AR_002</t>
-  </si>
-  <si>
-    <t>Lady2</t>
-  </si>
-  <si>
-    <t>Raga2</t>
-  </si>
-  <si>
-    <t>raga2@yopmail.com</t>
+    <t>TC_NA_001</t>
+  </si>
+  <si>
+    <t>New account creation</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>roy@yopmail.com</t>
+  </si>
+  <si>
+    <t>roy@123</t>
+  </si>
+  <si>
+    <t>TC_NA_002</t>
+  </si>
+  <si>
+    <t>Miller2</t>
+  </si>
+  <si>
+    <t>roy2@yopmail.com</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>Toy2</t>
   </si>
 </sst>
 </file>
@@ -468,49 +468,49 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{A694C5EB-FC5C-413C-B762-F3663F4F84FE}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{9757BE41-977C-4275-A2A1-8A34FA6E7C33}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{E12B992E-DBC8-4FBB-B35D-B2C7A58B949F}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{08292E5A-638F-473D-8571-F621BB9F49CC}"/>
-    <hyperlink ref="F3" r:id="rId5" xr:uid="{551FC2F0-5B28-49AA-894A-D82692026416}"/>
-    <hyperlink ref="G3" r:id="rId6" xr:uid="{24304149-8579-485C-AE3F-43DCE0EC1158}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{BF467897-B0FA-4B49-8A52-CCA29E80CEE4}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{A3C480EC-A4F2-4655-8BD2-3592764236BB}"/>
+    <hyperlink ref="G2" r:id="rId3" xr:uid="{B55309C7-FFF3-4659-B7FF-064D3E6BFBA2}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{6A4BEA47-95CA-4609-8C5F-E4D28CD68AF5}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{71C67E1C-BBAC-49A2-9A15-6541D805EF22}"/>
+    <hyperlink ref="G3" r:id="rId6" xr:uid="{7B4DBBE5-A4B5-4089-A3CF-ED1AFE74266C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>